<commit_message>
add coho figs and filter chinook figs
</commit_message>
<xml_diff>
--- a/Metrics/Temperature Descriptors.xlsx
+++ b/Metrics/Temperature Descriptors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GitHub\Temperature_Data\Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9659E621-604D-495A-B9B0-7AC3860BA3E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71890863-A564-4DFB-A0A2-178C36C87AE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30630" yWindow="1020" windowWidth="22845" windowHeight="14160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="1185" windowWidth="22845" windowHeight="14160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README - sheet desciptions" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="262">
   <si>
     <t>Description</t>
   </si>
@@ -850,12 +850,30 @@
   <si>
     <t>NOTE: Reduced list of 11 are highlighted</t>
   </si>
+  <si>
+    <t>Focus on:</t>
+  </si>
+  <si>
+    <t>change metrics that capture historic period</t>
+  </si>
+  <si>
+    <t>metrics specific to life-histories</t>
+  </si>
+  <si>
+    <t>threshold metrics for future only</t>
+  </si>
+  <si>
+    <t>degree days for rearing period</t>
+  </si>
+  <si>
+    <t>timing of warmest temperatures and increased interannual variation - shifting curve</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,6 +904,14 @@
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -947,7 +973,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -995,9 +1021,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1014,6 +1037,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2887,12 +2916,12 @@
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -4778,10 +4807,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5126,63 +5155,63 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="20" t="s">
+    <row r="20" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="20" t="s">
+    <row r="21" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="20" t="s">
+    <row r="22" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="19" t="s">
         <v>250</v>
       </c>
     </row>
@@ -5246,83 +5275,83 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="20" t="s">
+    <row r="26" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="19" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="20" t="s">
+    <row r="27" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="20" t="s">
+      <c r="D27" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="19" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="20" t="s">
+    <row r="28" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="19" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="20" t="s">
+    <row r="29" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D29" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="20" t="s">
+      <c r="D29" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5446,54 +5475,54 @@
         <v>249</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+    <row r="36" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="22" t="s">
+      <c r="D36" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+    <row r="37" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="D37" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="22" t="s">
+      <c r="D37" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+    <row r="38" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="24" t="s">
+      <c r="D38" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="23" t="s">
         <v>109</v>
       </c>
     </row>
@@ -5554,118 +5583,148 @@
         <v>251</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+    <row r="42" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="D42" s="25" t="s">
+      <c r="D42" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="26" t="s">
+      <c r="E42" s="25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+    <row r="43" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="26" t="s">
+      <c r="D43" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E43" s="25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+    <row r="44" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="26" t="s">
+      <c r="D44" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E44" s="26" t="s">
+      <c r="E44" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F44" s="26" t="s">
+      <c r="F44" s="25" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+    <row r="45" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D45" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="26" t="s">
+      <c r="D45" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="26" t="s">
+      <c r="F45" s="25" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+    <row r="46" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D46" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E46" s="26" t="s">
+      <c r="E46" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F46" s="26" t="s">
+      <c r="F46" s="25" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+    <row r="47" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="26" t="s">
+      <c r="D47" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="26" t="s">
+      <c r="E47" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F47" s="26" t="s">
+      <c r="F47" s="25" t="s">
         <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="25" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="25" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>